<commit_message>
Input File was Changed
スイッチの入れ方に修正を加えました。
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACS-NOSE\ANAtrial_nose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5E1851-4590-4B01-B9B5-4DDDB9908FA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0582BA-1476-48EE-BFDA-0508B5162425}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="URL" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>ascii</t>
     <phoneticPr fontId="1"/>
@@ -176,9 +176,6 @@
     <t>http://monoist.atmarkit.co.jp/</t>
   </si>
   <si>
-    <t>https://newswitch.jp/</t>
-  </si>
-  <si>
     <t>URL</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -265,14 +262,6 @@
     <t>VR広告</t>
   </si>
   <si>
-    <t>1: Run</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0: Not Run</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>1: HTTrack</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -281,10 +270,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>RunSwitch</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>WebName</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -293,23 +278,43 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ProgramSwitch</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2: Ctrl+S</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0: Not save</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0:</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2: ANA2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CrawlSwitch</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://newswitch.jp/index/searchdo?keyword=(keyword)&amp;x=0&amp;y=0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0: Not Save</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1: Save</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0: Not Crawl</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SavingPage</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1: Crawl</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CrawlingPage</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -342,7 +347,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,6 +357,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -389,12 +400,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -678,43 +717,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="12.5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.75" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="129.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="2"/>
+    <col min="3" max="5" width="11.75" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="129.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="18">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="18">
       <c r="A1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>75</v>
+      <c r="C1" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -722,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
@@ -730,11 +770,14 @@
       <c r="E2" s="4">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -742,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -750,11 +793,14 @@
       <c r="E3" s="4">
         <v>1</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -762,7 +808,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -770,11 +816,14 @@
       <c r="E4" s="4">
         <v>1</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -782,7 +831,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -790,31 +839,37 @@
       <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="4">
         <v>0</v>
       </c>
       <c r="D6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="4">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -822,19 +877,22 @@
         <v>0</v>
       </c>
       <c r="C7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="4">
-        <v>1</v>
-      </c>
-      <c r="F7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -842,7 +900,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
@@ -850,11 +908,14 @@
       <c r="E8" s="4">
         <v>1</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -862,19 +923,22 @@
         <v>0</v>
       </c>
       <c r="C9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
       </c>
       <c r="E9" s="4">
-        <v>2</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
+        <v>2</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -882,19 +946,22 @@
         <v>0</v>
       </c>
       <c r="C10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
       </c>
       <c r="E10" s="4">
-        <v>2</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
+        <v>2</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -902,19 +969,22 @@
         <v>0</v>
       </c>
       <c r="C11" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="4">
         <v>2</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="F11" s="4">
+        <v>2</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
@@ -922,19 +992,22 @@
         <v>0</v>
       </c>
       <c r="C12" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
       </c>
       <c r="E12" s="4">
-        <v>2</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
+        <v>2</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -942,19 +1015,22 @@
         <v>0</v>
       </c>
       <c r="C13" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
       </c>
       <c r="E13" s="4">
-        <v>2</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4">
+        <v>2</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="4" t="s">
         <v>0</v>
       </c>
@@ -962,19 +1038,22 @@
         <v>0</v>
       </c>
       <c r="C14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="4">
-        <v>2</v>
-      </c>
-      <c r="F14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4">
+        <v>2</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
         <v>1</v>
       </c>
@@ -982,19 +1061,22 @@
         <v>0</v>
       </c>
       <c r="C15" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D15" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="4">
-        <v>2</v>
-      </c>
-      <c r="F15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4">
+        <v>2</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16" s="4" t="s">
         <v>2</v>
       </c>
@@ -1002,19 +1084,22 @@
         <v>0</v>
       </c>
       <c r="C16" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D16" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" s="4" t="s">
         <v>3</v>
       </c>
@@ -1022,19 +1107,22 @@
         <v>0</v>
       </c>
       <c r="C17" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D17" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="4">
-        <v>2</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4">
+        <v>2</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
@@ -1042,19 +1130,22 @@
         <v>0</v>
       </c>
       <c r="C18" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D18" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="4">
         <v>1</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7">
       <c r="A19" s="4" t="s">
         <v>5</v>
       </c>
@@ -1062,19 +1153,22 @@
         <v>0</v>
       </c>
       <c r="C19" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D19" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="4">
-        <v>2</v>
-      </c>
-      <c r="F19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4">
+        <v>2</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7">
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
@@ -1082,19 +1176,22 @@
         <v>0</v>
       </c>
       <c r="C20" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D20" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E20" s="4">
-        <v>1</v>
-      </c>
-      <c r="F20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
@@ -1102,19 +1199,22 @@
         <v>0</v>
       </c>
       <c r="C21" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D21" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E21" s="4">
-        <v>1</v>
-      </c>
-      <c r="F21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7">
       <c r="A22" s="4" t="s">
         <v>8</v>
       </c>
@@ -1122,19 +1222,22 @@
         <v>0</v>
       </c>
       <c r="C22" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D22" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22" s="4">
-        <v>2</v>
-      </c>
-      <c r="F22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4">
+        <v>2</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23" s="4" t="s">
         <v>9</v>
       </c>
@@ -1142,19 +1245,22 @@
         <v>0</v>
       </c>
       <c r="C23" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D23" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" s="4">
         <v>1</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="4">
+        <v>1</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7">
       <c r="A24" s="4" t="s">
         <v>10</v>
       </c>
@@ -1162,19 +1268,22 @@
         <v>0</v>
       </c>
       <c r="C24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D24" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E24" s="4">
         <v>2</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="F24" s="4">
+        <v>2</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="4" t="s">
         <v>11</v>
       </c>
@@ -1182,53 +1291,61 @@
         <v>0</v>
       </c>
       <c r="C25" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D25" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" s="4">
-        <v>2</v>
-      </c>
-      <c r="F25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="4">
+        <v>2</v>
+      </c>
+      <c r="G25" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7">
       <c r="B26" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="C26" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="B27" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="E27" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="D28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="C28" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="B2:D25">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="B2:C25">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:E25">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1246,92 +1363,92 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Input.xlsx Change for GetHref
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACS-NOSE\ANAtrial_nose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0582BA-1476-48EE-BFDA-0508B5162425}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8FD988-C6FC-48B6-9EB6-02810F253DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="233">
   <si>
     <t>ascii</t>
     <phoneticPr fontId="1"/>
@@ -124,10 +124,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>pageNum</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>https://ascii.jp/search/?cx=004761988070997154717%3Akxpchiveidg&amp;cof=FORID%3A11&amp;q=(keyword)&amp;sa=%E6%A4%9C%E7%B4%A2</t>
   </si>
   <si>
@@ -180,26 +176,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>https://robotstart.info/?paged=1&amp;s=(keyword)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>https://sorae.info/?s=(keyword)&amp;paged=1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>https://techable.jp/page/1/?s=(keyword)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>https://wirelesswire.jp/page/1/?s=(keyword)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>https://www.moguravr.com/page/1/?s=(keyword)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>http://kensaku.itmedia.co.jp/?q=(keyword)&amp;start=0&amp;sort=desc&amp;ch=&amp;path=http%3A%2F%2Fwww.itmedia.co.jp%2F</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -306,15 +282,553 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>SavingPage</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>1: Crawl</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>CrawlingPage</t>
+    <t>Class_Title</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Class_Href</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Class_PostDate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Class_Source</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Class_Content</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>replace_nxt_p</t>
+  </si>
+  <si>
+    <t>case_display</t>
+  </si>
+  <si>
+    <t>class_tr_dl</t>
+  </si>
+  <si>
+    <t>click_sort</t>
+  </si>
+  <si>
+    <t>class_gsc_cursor_page</t>
+  </si>
+  <si>
+    <t>#main &gt; div &gt; article &gt; a</t>
+  </si>
+  <si>
+    <t>#main &gt; div &gt; article &gt; a &gt; section &gt; h1</t>
+  </si>
+  <si>
+    <t>#main &gt; article &gt; header &gt; p &gt; time</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>#main &gt; article &gt; section</t>
+  </si>
+  <si>
+    <t>page/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai</t>
+  </si>
+  <si>
+    <t>?s=</t>
+  </si>
+  <si>
+    <t>#search_results &gt; section &gt; h2 &gt; a</t>
+  </si>
+  <si>
+    <t>#article &gt; div.cntimage &gt; div &gt; time</t>
+  </si>
+  <si>
+    <t>#article &gt; div.cntimage &gt; p</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>https://gigazine.net</t>
+  </si>
+  <si>
+    <t>stp=1</t>
+  </si>
+  <si>
+    <t>body &gt; main &gt; div &gt; div &gt; div &gt; div &gt; div &gt; h4 &gt; a</t>
+  </si>
+  <si>
+    <t>body &gt; main &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; p.releae-up-date</t>
+  </si>
+  <si>
+    <t>body &gt; main &gt; div &gt; div &gt; div &gt; div.release-body &gt; p:last-child</t>
+  </si>
+  <si>
+    <t>body &gt; main &gt; div &gt; div &gt; div &gt; div.release-body &gt; p</t>
+  </si>
+  <si>
+    <t>&amp;page=</t>
+  </si>
+  <si>
+    <t>https://kyodonewsprwire.jp</t>
+  </si>
+  <si>
+    <t>body &gt; div.wrapper &gt; div.container &gt; div.body &gt; main &gt; section &gt; div &gt; section &gt; div &gt; h3 &gt; a</t>
+  </si>
+  <si>
+    <t>body &gt; div.wrapper &gt; div.container &gt; div.body &gt; main &gt; div.article-author &gt; div &gt; p</t>
+  </si>
+  <si>
+    <t>body &gt; div.wrapper &gt; div.container &gt; div.body &gt; main &gt; article &gt; div &gt; p</t>
+  </si>
+  <si>
+    <t>page=</t>
+  </si>
+  <si>
+    <t>https://news.mynavi.jp</t>
+  </si>
+  <si>
+    <t>commit=</t>
+  </si>
+  <si>
+    <t>#itemThumbnailView&gt;div&gt;article&gt;h3&gt;a</t>
+  </si>
+  <si>
+    <t>#main &gt; div &gt; article &gt; div &gt; header &gt; div &gt; time</t>
+  </si>
+  <si>
+    <t>#main &gt; div &gt; article &gt; div &gt; div &gt; div</t>
+  </si>
+  <si>
+    <t>https://prtimes.jp</t>
+  </si>
+  <si>
+    <t>#contents &gt; div.main &gt; a</t>
+  </si>
+  <si>
+    <t>#contents &gt; div.main &gt; a &gt; article &gt; h4</t>
+  </si>
+  <si>
+    <t>#contents &gt; div &gt; article &gt; div.article_date &gt; time</t>
+  </si>
+  <si>
+    <t>#contents &gt; div &gt; article &gt; div.article_text</t>
+  </si>
+  <si>
+    <t>https://newswitch.jp</t>
+  </si>
+  <si>
+    <t>&amp;x=10&amp;y=15</t>
+  </si>
+  <si>
+    <t>#content &gt; div &gt; div &gt; div &gt; h4 &gt; a</t>
+  </si>
+  <si>
+    <t>#content &gt; div &gt; div &gt; div &gt; h4</t>
+  </si>
+  <si>
+    <t>body &gt; div&gt; div &gt; div &gt; div&gt; div.date_top</t>
+  </si>
+  <si>
+    <t>body &gt; div&gt; div &gt; div &gt; div&gt; div &gt; p</t>
+  </si>
+  <si>
+    <t>https://roboteer-tokyo.com</t>
+  </si>
+  <si>
+    <t>#main-content &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; ul &gt; div &gt; a</t>
+  </si>
+  <si>
+    <t>#main-content &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; ul &gt; div &gt; a&gt;li&gt;article&gt;div&gt;header&gt;h4</t>
+  </si>
+  <si>
+    <t>header &gt; div &gt; div&gt; span.entry-date</t>
+  </si>
+  <si>
+    <t>div.elements-box &gt; p</t>
+  </si>
+  <si>
+    <t>?paged=</t>
+  </si>
+  <si>
+    <t>https://robotstart.info</t>
+  </si>
+  <si>
+    <t>#post_list &gt; li&gt; div &gt; h4 &gt; a</t>
+  </si>
+  <si>
+    <t>#post_list &gt; li&gt; div &gt; h4</t>
+  </si>
+  <si>
+    <t>div&gt;div&gt;div &gt;ul&gt;li.date</t>
+  </si>
+  <si>
+    <t>#left_col &gt; div.post.clearfix &gt; p</t>
+  </si>
+  <si>
+    <t>&amp;paged=</t>
+  </si>
+  <si>
+    <t>https://sorae.info</t>
+  </si>
+  <si>
+    <t>body &gt; div&gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div&gt; section &gt; a</t>
+  </si>
+  <si>
+    <t>body &gt; div&gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div&gt; section &gt; a&gt;div&gt;div&gt;h3</t>
+  </si>
+  <si>
+    <t>body &gt; div &gt; div &gt; div&gt; div &gt; div &gt; div&gt; time</t>
+  </si>
+  <si>
+    <t>body &gt; div &gt; div  div &gt; div &gt; div.te-cms-body</t>
+  </si>
+  <si>
+    <t>https://techable.jp</t>
+  </si>
+  <si>
+    <t>body &gt; div&gt; div &gt; div&gt; ul &gt; li &gt; article &gt; p &gt; a</t>
+  </si>
+  <si>
+    <t>body &gt; div&gt; div &gt; div&gt; ul &gt; li &gt; article &gt; p</t>
+  </si>
+  <si>
+    <t>body &gt; div.wrapBody &gt; div &gt; article &gt; div &gt; p.block3__date</t>
+  </si>
+  <si>
+    <t>body &gt; div &gt; div &gt; div &gt; div &gt; div.wysiwyg</t>
+  </si>
+  <si>
+    <t>https://wirelesswire.jp</t>
+  </si>
+  <si>
+    <t>body &gt; div.mg-main &gt; div &gt; div &gt; div.column.is-8.mg-content &gt; a</t>
+  </si>
+  <si>
+    <t>body &gt; div.mg-main &gt; div &gt; div &gt; div.column.is-8.mg-content &gt; a &gt; div &gt; div &gt; h4</t>
+  </si>
+  <si>
+    <t>body &gt; div.mg-main &gt; div &gt; div &gt; div.column.is-8.mg-content &gt; div.mg-article &gt; article &gt; p</t>
+  </si>
+  <si>
+    <t>body &gt; div.mg-main &gt; div &gt; div &gt; div.column.is-8.mg-content &gt; div.mg-article &gt; article &gt; div.mg-article-content &gt; p</t>
+  </si>
+  <si>
+    <t>https://www.moguravr.com</t>
+  </si>
+  <si>
+    <t>#___gcse_0 &gt; div &gt; div &gt; div &gt; div.gsc-wrapper &gt; div.gsc-resultsbox-visible &gt; div &gt; div &gt; div.gsc-webResult.gsc-result &gt; div.gs-webResult.gs-result &gt; div.gsc-table-result &gt; div.gsc-table-cell-snippet-close &gt; div &gt; a,#___gcse_0 &gt; div &gt; div &gt; div &gt; div.gsc-wrapper &gt; div.gsc-resultsbox-visible &gt; div &gt; div &gt; div.gsc-expansionArea &gt; div &gt; div.gs-webResult.gs-result &gt; div.gsc-table-result &gt; div.gsc-table-cell-snippet-close &gt; div &gt; a</t>
+  </si>
+  <si>
+    <t>#articleHead &gt; div.artdata &gt; p.date</t>
+  </si>
+  <si>
+    <t>#mainC &gt; p</t>
+  </si>
+  <si>
+    <t>https://ascii.jp</t>
+  </si>
+  <si>
+    <t>gsc-cursor-page</t>
+  </si>
+  <si>
+    <t>#module-engadget-search-streams &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; ul &gt; li &gt; a</t>
+  </si>
+  <si>
+    <t>#module-engadget-search-streams &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; ul &gt; li &gt; a &gt; div &gt; div &gt; div &gt; h2</t>
+  </si>
+  <si>
+    <t>body &gt; div &gt; div &gt; div &gt; main &gt; div &gt; div.grid.flex.fixto_top &gt; div &gt; article &gt; header &gt; div &gt; div &gt; section &gt; div &gt; div &gt; div &gt; div.th-meta</t>
+  </si>
+  <si>
+    <t>#page_body &gt; div &gt; div &gt; div &gt; div &gt; footer &gt; div &gt; div &gt; div &gt; section &gt; div:nth-child(2) &gt; span.th-meta</t>
+  </si>
+  <si>
+    <t>#page_body &gt; div &gt; div &gt; div&gt; div &gt; div &gt; div &gt; div</t>
+  </si>
+  <si>
+    <t>stp=</t>
+  </si>
+  <si>
+    <t>https://japanese.engadget.com</t>
+  </si>
+  <si>
+    <t>page-link</t>
+  </si>
+  <si>
+    <t>#searchResultList &gt; ul &gt; li &gt; article &gt; div &gt; h3 &gt; a</t>
+  </si>
+  <si>
+    <t>body &gt; main &gt; div &gt; article &gt; ul:nth-child(4) &gt; li &gt; time</t>
+  </si>
+  <si>
+    <t>body &gt; main &gt; div &gt; article &gt; div.p-post-content</t>
+  </si>
+  <si>
+    <t>https://www.gizmodo.jp</t>
+  </si>
+  <si>
+    <t>#popin_content_main &gt; ul &gt; li &gt; div.popIn_ArticleTitle &gt; a</t>
+  </si>
+  <si>
+    <t>#masterContents &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div.inner &gt; span#update</t>
+  </si>
+  <si>
+    <t>#masterContents &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div.inner &gt; p</t>
+  </si>
+  <si>
+    <t>&amp;start=</t>
+  </si>
+  <si>
+    <t>https://www.itmedia.co.jp</t>
+  </si>
+  <si>
+    <t>popIn_NavigatorBox</t>
+  </si>
+  <si>
+    <t>#___gcse_0 &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div.gsc-thumbnail-inside &gt; div &gt; a,#___gcse_0 &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div.gsc-thumbnail-inside &gt; div &gt; a</t>
+  </si>
+  <si>
+    <t>#leaf-column &gt; div &gt; div &gt; div.leaf-headline-inner &gt; span.date &gt; a</t>
+  </si>
+  <si>
+    <t>#leaf-column &gt; div.leaf-article-inner.block_story &gt; div &gt; p</t>
+  </si>
+  <si>
+    <t>https://japan.cnet.com</t>
+  </si>
+  <si>
+    <t>#___gcse_0 &gt; div &gt; div &gt; div &gt; div &gt; div&gt; div &gt; div &gt; div &gt; div &gt; div &gt; div&gt; div &gt; a</t>
+  </si>
+  <si>
+    <t>#cmsDate &gt; div &gt; span#update</t>
+  </si>
+  <si>
+    <t>#cmsBody &gt; div &gt; p</t>
+  </si>
+  <si>
+    <t>https://monoist.atmarkit.co.jp</t>
+  </si>
+  <si>
+    <t>/?s=</t>
+  </si>
+  <si>
+    <t>body &gt; div &gt; div &gt; div &gt; div&gt; div &gt; a</t>
+  </si>
+  <si>
+    <t>#changeArea &gt; p.date</t>
+  </si>
+  <si>
+    <t>#changeArea &gt; div &gt; p</t>
+  </si>
+  <si>
+    <t>https://www.nikkan.co.jp</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>body &gt; div &gt; main &gt; div &gt; div&gt; div &gt; div&gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div&gt; div&gt; h3 &gt; a</t>
+  </si>
+  <si>
+    <t>body &gt; div &gt; main &gt; div &gt; div&gt; div &gt; div&gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div&gt; div&gt; h3</t>
+  </si>
+  <si>
+    <t>#CONTENTS_MAIN &gt; div &gt; dl &gt; dd</t>
+  </si>
+  <si>
+    <t>#CONTENTS_MAIN &gt; div&gt; div&gt; p</t>
+  </si>
+  <si>
+    <t>https://www.nikkei.com/</t>
+  </si>
+  <si>
+    <t>#___gcse_0 &gt; div &gt; div &gt; div &gt; div.gsc-wrapper &gt; div &gt; div &gt; div &gt; div&gt; div &gt; div.gsc-thumbnail-inside &gt; div &gt; a,#___gcse_0 &gt; div &gt; div &gt; div &gt; div.gsc-wrapper &gt; div &gt; div&gt; div &gt; div &gt; div&gt; div&gt; div.gsc-thumbnail-inside &gt; div &gt; a</t>
+  </si>
+  <si>
+    <t>body &gt; div&gt; main &gt; header &gt; time</t>
+  </si>
+  <si>
+    <t>body &gt; div &gt; main &gt; div&gt; article&gt;p</t>
+  </si>
+  <si>
+    <t>https://response.jp</t>
+  </si>
+  <si>
+    <t>#wrapper &gt; div &gt; article &gt; div &gt; section &gt; ul &gt; li &gt; div&gt; h3 &gt; a</t>
+  </si>
+  <si>
+    <t>#wrapper &gt; div &gt; article &gt; div &gt; section &gt; ul &gt; li &gt; div&gt; h3</t>
+  </si>
+  <si>
+    <t>#wrapper &gt; div &gt; article &gt; header &gt; div.articleHeaderTop &gt; time</t>
+  </si>
+  <si>
+    <t>#wrapper &gt; div &gt; article &gt; div</t>
+  </si>
+  <si>
+    <t>&amp;p=</t>
+  </si>
+  <si>
+    <t>https://tech.nikkeibp.co.jp</t>
+  </si>
+  <si>
+    <t>#wrapper &gt; div &gt; article &gt; div &gt; nav &gt; ul &gt; li</t>
+  </si>
+  <si>
+    <t>#st-results-container &gt; li &gt; div &gt; div &gt; h2 &gt; a</t>
+  </si>
+  <si>
+    <t>body &gt; div.fluid &gt; article &gt; div &gt; div.l-main-container &gt; div &gt; header &gt; div.title-left &gt; div.byline &gt; time</t>
+  </si>
+  <si>
+    <t>body &gt; div&gt; article &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div &gt; div&gt;p</t>
+  </si>
+  <si>
+    <t>#___gcse_0 &gt; div &gt; div &gt; div &gt; div &gt; div&gt; div &gt; div &gt; div&gt; div &gt; div&gt; div &gt; div.gs-title &gt; a</t>
+  </si>
+  <si>
+    <t>div &gt; article &gt; header &gt; time</t>
+  </si>
+  <si>
+    <t>main#main-article-detail &gt; div &gt; div.contents-block &gt; article.article-detail &gt; p</t>
+  </si>
+  <si>
+    <t>https://wired.jp</t>
+  </si>
+  <si>
+    <t>https://jp.techcrunch.com</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>click_Search</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>class_Next_page</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Domain</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CrawlMethod</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SaveMethod</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>20件</t>
+    <rPh sb="2" eb="3">
+      <t>ケン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>25件</t>
+    <rPh sb="2" eb="3">
+      <t>ケン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>30件</t>
+    <rPh sb="2" eb="3">
+      <t>ケン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>21件</t>
+    <rPh sb="2" eb="3">
+      <t>ケン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>15件</t>
+    <rPh sb="2" eb="3">
+      <t>ケン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>10件</t>
+    <rPh sb="2" eb="3">
+      <t>ケン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>14件</t>
+    <rPh sb="2" eb="3">
+      <t>ケン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>16件</t>
+    <rPh sb="2" eb="3">
+      <t>ケン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>備考(1ページ目の表示アイテム数)</t>
+    <rPh sb="0" eb="2">
+      <t>ビコウ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>メ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>スウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>50件</t>
+    <rPh sb="2" eb="3">
+      <t>ケン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PageNum</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://robotstart.info/?paged=(pagenum)&amp;s=(keyword)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://sorae.info/?s=(keyword)&amp;paged=(pagenum)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://techable.jp/page/(pagenum)/?s=(keyword)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://wirelesswire.jp/page/(pagenum)/?s=(keyword)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://www.moguravr.com/page/(pagenum)/?s=(keyword)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -405,21 +919,7 @@
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -437,7 +937,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -717,7 +1217,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -727,39 +1227,83 @@
     <col min="2" max="2" width="11.75" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="11.75" style="2" customWidth="1"/>
     <col min="6" max="6" width="10.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="129.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="2"/>
+    <col min="7" max="7" width="56.75" style="2" customWidth="1"/>
+    <col min="8" max="14" width="9" style="2"/>
+    <col min="15" max="15" width="30.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="18">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="18">
       <c r="A1" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="J1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="S1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="4">
         <v>0</v>
@@ -774,10 +1318,50 @@
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>33</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="M2" s="4">
+        <v>2</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>20</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S2" s="4">
+        <v>0</v>
+      </c>
+      <c r="T2" s="4"/>
+      <c r="U2" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -797,10 +1381,50 @@
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>34</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M3" s="4">
+        <v>1</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>50</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S3" s="4">
+        <v>0</v>
+      </c>
+      <c r="T3" s="4"/>
+      <c r="U3" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -820,10 +1444,50 @@
         <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>35</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="M4" s="4">
+        <v>2</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>25</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S4" s="4">
+        <v>0</v>
+      </c>
+      <c r="T4" s="4"/>
+      <c r="U4" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -843,10 +1507,50 @@
         <v>1</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>36</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="M5" s="4">
+        <v>1</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>30</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S5" s="4">
+        <v>0</v>
+      </c>
+      <c r="T5" s="4"/>
+      <c r="U5" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -866,10 +1570,50 @@
         <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>68</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="M6" s="4">
+        <v>1</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>21</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S6" s="4">
+        <v>0</v>
+      </c>
+      <c r="T6" s="4"/>
+      <c r="U6" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -889,10 +1633,50 @@
         <v>1</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>37</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="M7" s="4">
+        <v>1</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>20</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S7" s="4">
+        <v>0</v>
+      </c>
+      <c r="T7" s="4"/>
+      <c r="U7" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -912,10 +1696,50 @@
         <v>1</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>38</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>10</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S8" s="4">
+        <v>0</v>
+      </c>
+      <c r="T8" s="4"/>
+      <c r="U8" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -935,10 +1759,50 @@
         <v>2</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>228</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>15</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S9" s="4">
+        <v>0</v>
+      </c>
+      <c r="T9" s="4"/>
+      <c r="U9" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -958,10 +1822,50 @@
         <v>2</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>229</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>10</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S10" s="4">
+        <v>0</v>
+      </c>
+      <c r="T10" s="4"/>
+      <c r="U10" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -981,10 +1885,50 @@
         <v>2</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>230</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="M11" s="4">
+        <v>2</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>14</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S11" s="4">
+        <v>0</v>
+      </c>
+      <c r="T11" s="4"/>
+      <c r="U11" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
@@ -1004,10 +1948,50 @@
         <v>2</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>231</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>20</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S12" s="4">
+        <v>0</v>
+      </c>
+      <c r="T12" s="4"/>
+      <c r="U12" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -1027,10 +2011,50 @@
         <v>2</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>232</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>16</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S13" s="4">
+        <v>0</v>
+      </c>
+      <c r="T13" s="4"/>
+      <c r="U13" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" s="4" t="s">
         <v>0</v>
       </c>
@@ -1050,56 +2074,182 @@
         <v>2</v>
       </c>
       <c r="G14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="M14" s="4">
+        <v>1</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>10</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S14" s="4">
+        <v>2</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4">
+        <v>2</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="4">
-        <v>0</v>
-      </c>
-      <c r="C15" s="4">
-        <v>0</v>
-      </c>
-      <c r="D15" s="4">
-        <v>2</v>
-      </c>
-      <c r="E15" s="4">
-        <v>1</v>
-      </c>
-      <c r="F15" s="4">
-        <v>2</v>
-      </c>
-      <c r="G15" s="4" t="s">
+      <c r="H15" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="M15" s="4">
+        <v>2</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>10</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S15" s="4">
+        <v>0</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="4">
-        <v>0</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4">
-        <v>2</v>
-      </c>
-      <c r="E16" s="4">
-        <v>1</v>
-      </c>
-      <c r="F16" s="4">
-        <v>1</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="M16" s="4">
+        <v>2</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>50</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S16" s="4">
+        <v>0</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" s="4" t="s">
         <v>3</v>
       </c>
@@ -1119,10 +2269,52 @@
         <v>2</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>41</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="M17" s="4">
+        <v>1</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>10</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S17" s="4">
+        <v>0</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
@@ -1142,10 +2334,52 @@
         <v>1</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>27</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="M18" s="4">
+        <v>1</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>10</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S18" s="4">
+        <v>2</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="U18" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" s="4" t="s">
         <v>5</v>
       </c>
@@ -1165,10 +2399,52 @@
         <v>2</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>39</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="M19" s="4">
+        <v>2</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>10</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S19" s="4">
+        <v>2</v>
+      </c>
+      <c r="T19" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="U19" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
@@ -1188,10 +2464,52 @@
         <v>1</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>28</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="M20" s="4">
+        <v>1</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>20</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S20" s="4">
+        <v>0</v>
+      </c>
+      <c r="T20" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="U20" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
@@ -1211,10 +2529,52 @@
         <v>1</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>29</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="M21" s="4">
+        <v>1</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>9</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S21" s="4">
+        <v>0</v>
+      </c>
+      <c r="T21" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="U21" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" s="4" t="s">
         <v>8</v>
       </c>
@@ -1234,10 +2594,52 @@
         <v>2</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>30</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="M22" s="4">
+        <v>1</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>0</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S22" s="4">
+        <v>0</v>
+      </c>
+      <c r="T22" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="U22" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23" s="4" t="s">
         <v>9</v>
       </c>
@@ -1257,10 +2659,52 @@
         <v>1</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>31</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="M23" s="4">
+        <v>1</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>20</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S23" s="4">
+        <v>0</v>
+      </c>
+      <c r="T23" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="U23" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" s="4" t="s">
         <v>10</v>
       </c>
@@ -1280,10 +2724,52 @@
         <v>2</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>42</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="M24" s="4">
+        <v>1</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="P24" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>10</v>
+      </c>
+      <c r="R24" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S24" s="4">
+        <v>1</v>
+      </c>
+      <c r="T24" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="U24" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25" s="4" t="s">
         <v>11</v>
       </c>
@@ -1303,49 +2789,96 @@
         <v>2</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>32</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M25" s="4">
+        <v>2</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="P25" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>10</v>
+      </c>
+      <c r="R25" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S25" s="4">
+        <v>2</v>
+      </c>
+      <c r="T25" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
       <c r="B26" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
       <c r="B27" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
       <c r="D28" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="B2:C25">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:E25">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F25">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1363,92 +2896,92 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update ANA2 (which can save temp1, temp2)
全サイトでtemp1,temp2を保存できるように調整しています。
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACS-NOSE\ANAtrial_nose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8FD988-C6FC-48B6-9EB6-02810F253DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B197C473-F157-4FBC-AF3B-766EB1C7ABA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="234">
   <si>
     <t>ascii</t>
     <phoneticPr fontId="1"/>
@@ -167,9 +167,6 @@
   </si>
   <si>
     <t>https://roboteer-tokyo.com/?s=(keyword)</t>
-  </si>
-  <si>
-    <t>http://monoist.atmarkit.co.jp/</t>
   </si>
   <si>
     <t>URL</t>
@@ -829,6 +826,14 @@
   </si>
   <si>
     <t>https://www.moguravr.com/page/(pagenum)/?s=(keyword)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://cse.google.co.jp/cse?cx=partner-pub-2201843946232317:9909425848&amp;q=(keyword)&amp;oq=(keyword)&amp;gs_l=partner-generic.3...9274.9387.0.10069.2.2.0.0.0.0.59.103.2.2.0.gsnos%2Cn%3D13...0.44j976j3..1ac.1.25.partner-generic..1.1.59.hWZNG5ZBd8A</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1235,67 +1240,67 @@
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" ht="18">
       <c r="A1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="D1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>216</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="T1" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="U1" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -1303,7 +1308,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="4">
         <v>0</v>
@@ -1312,7 +1317,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="4">
         <v>1</v>
@@ -1321,44 +1326,46 @@
         <v>33</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="K2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4">
+        <v>2</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="M2" s="4">
-        <v>2</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="Q2" s="4">
         <v>20</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S2" s="4">
         <v>0</v>
       </c>
-      <c r="T2" s="4"/>
+      <c r="T2" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="U2" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -1384,44 +1391,46 @@
         <v>34</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4">
+        <v>1</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="M3" s="4">
-        <v>1</v>
-      </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="Q3" s="4">
         <v>50</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S3" s="4">
         <v>0</v>
       </c>
-      <c r="T3" s="4"/>
+      <c r="T3" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="U3" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -1447,44 +1456,46 @@
         <v>35</v>
       </c>
       <c r="H4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="M4" s="4">
+        <v>2</v>
+      </c>
+      <c r="N4" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="M4" s="4">
-        <v>2</v>
-      </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="O4" s="4" t="s">
-        <v>102</v>
-      </c>
       <c r="P4" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q4" s="4">
         <v>25</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S4" s="4">
         <v>0</v>
       </c>
-      <c r="T4" s="4"/>
+      <c r="T4" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="U4" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -1510,44 +1521,46 @@
         <v>36</v>
       </c>
       <c r="H5" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="4">
+        <v>1</v>
+      </c>
+      <c r="N5" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="M5" s="4">
-        <v>1</v>
-      </c>
-      <c r="N5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="Q5" s="4">
         <v>30</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S5" s="4">
         <v>0</v>
       </c>
-      <c r="T5" s="4"/>
+      <c r="T5" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="U5" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -1570,47 +1583,49 @@
         <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H6" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="K6" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L6" s="4" t="s">
+      <c r="M6" s="4">
+        <v>1</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="O6" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="M6" s="4">
-        <v>1</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="O6" s="4" t="s">
+      <c r="P6" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="Q6" s="4">
         <v>21</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S6" s="4">
         <v>0</v>
       </c>
-      <c r="T6" s="4"/>
+      <c r="T6" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="U6" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -1636,44 +1651,46 @@
         <v>37</v>
       </c>
       <c r="H7" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="J7" s="4" t="s">
+      <c r="K7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L7" s="4" t="s">
+      <c r="M7" s="4">
+        <v>1</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O7" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="M7" s="4">
-        <v>1</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>112</v>
-      </c>
       <c r="P7" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q7" s="4">
         <v>20</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S7" s="4">
         <v>0</v>
       </c>
-      <c r="T7" s="4"/>
+      <c r="T7" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="U7" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -1699,44 +1716,46 @@
         <v>38</v>
       </c>
       <c r="H8" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="K8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L8" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L8" s="4" t="s">
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O8" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="4">
-        <v>1</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>123</v>
-      </c>
       <c r="P8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q8" s="4">
         <v>10</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S8" s="4">
         <v>0</v>
       </c>
-      <c r="T8" s="4"/>
+      <c r="T8" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="U8" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1759,47 +1778,49 @@
         <v>2</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H9" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="J9" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="K9" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L9" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="K9" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L9" s="4" t="s">
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
+      <c r="N9" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="M9" s="4">
-        <v>1</v>
-      </c>
-      <c r="N9" s="4" t="s">
+      <c r="O9" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="O9" s="4" t="s">
-        <v>129</v>
-      </c>
       <c r="P9" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q9" s="4">
         <v>15</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S9" s="4">
         <v>0</v>
       </c>
-      <c r="T9" s="4"/>
+      <c r="T9" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="U9" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -1822,47 +1843,49 @@
         <v>2</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H10" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="J10" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="K10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="K10" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L10" s="4" t="s">
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+      <c r="N10" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="M10" s="4">
-        <v>1</v>
-      </c>
-      <c r="N10" s="4" t="s">
+      <c r="O10" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="O10" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="P10" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q10" s="4">
         <v>10</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S10" s="4">
         <v>0</v>
       </c>
-      <c r="T10" s="4"/>
+      <c r="T10" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="U10" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1885,47 +1908,49 @@
         <v>2</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H11" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="K11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="K11" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L11" s="4" t="s">
+      <c r="M11" s="4">
+        <v>2</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="O11" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="M11" s="4">
-        <v>2</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>140</v>
-      </c>
       <c r="P11" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q11" s="4">
         <v>14</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S11" s="4">
         <v>0</v>
       </c>
-      <c r="T11" s="4"/>
+      <c r="T11" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="U11" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1948,47 +1973,49 @@
         <v>2</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H12" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="J12" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="K12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="K12" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L12" s="4" t="s">
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="O12" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="M12" s="4">
-        <v>1</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>145</v>
-      </c>
       <c r="P12" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q12" s="4">
         <v>20</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S12" s="4">
         <v>0</v>
       </c>
-      <c r="T12" s="4"/>
+      <c r="T12" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="U12" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -2011,47 +2038,49 @@
         <v>2</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H13" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="J13" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="K13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="K13" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L13" s="4" t="s">
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="O13" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="M13" s="4">
-        <v>1</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>150</v>
-      </c>
       <c r="P13" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q13" s="4">
         <v>16</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S13" s="4">
         <v>0</v>
       </c>
-      <c r="T13" s="4"/>
+      <c r="T13" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="U13" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -2077,46 +2106,46 @@
         <v>24</v>
       </c>
       <c r="H14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="J14" s="4" t="s">
+      <c r="K14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L14" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="K14" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L14" s="4" t="s">
+      <c r="M14" s="4">
+        <v>1</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O14" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="M14" s="4">
-        <v>1</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>154</v>
-      </c>
       <c r="P14" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q14" s="4">
         <v>10</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S14" s="4">
         <v>2</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -2142,46 +2171,46 @@
         <v>25</v>
       </c>
       <c r="H15" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="J15" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="K15" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="L15" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="M15" s="4">
+        <v>2</v>
+      </c>
+      <c r="N15" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="M15" s="4">
-        <v>2</v>
-      </c>
-      <c r="N15" s="4" t="s">
+      <c r="O15" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="O15" s="4" t="s">
-        <v>162</v>
-      </c>
       <c r="P15" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q15" s="4">
         <v>10</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S15" s="4">
         <v>0</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -2207,46 +2236,46 @@
         <v>26</v>
       </c>
       <c r="H16" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="I16" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="J16" s="4" t="s">
+      <c r="K16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="K16" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L16" s="4" t="s">
+      <c r="M16" s="4">
+        <v>2</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O16" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="M16" s="4">
-        <v>2</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>167</v>
-      </c>
       <c r="P16" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q16" s="4">
         <v>50</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S16" s="4">
         <v>0</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -2254,7 +2283,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="4">
         <v>0</v>
@@ -2269,49 +2298,49 @@
         <v>2</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H17" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="J17" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="I17" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="J17" s="4" t="s">
+      <c r="K17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="K17" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L17" s="4" t="s">
+      <c r="M17" s="4">
+        <v>1</v>
+      </c>
+      <c r="N17" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="M17" s="4">
-        <v>1</v>
-      </c>
-      <c r="N17" s="4" t="s">
+      <c r="O17" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="O17" s="4" t="s">
-        <v>172</v>
-      </c>
       <c r="P17" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q17" s="4">
         <v>10</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S17" s="4">
         <v>0</v>
       </c>
       <c r="T17" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -2337,46 +2366,46 @@
         <v>27</v>
       </c>
       <c r="H18" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="J18" s="4" t="s">
+      <c r="K18" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L18" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="K18" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L18" s="4" t="s">
+      <c r="M18" s="4">
+        <v>1</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O18" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="M18" s="4">
-        <v>1</v>
-      </c>
-      <c r="N18" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="O18" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="P18" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q18" s="4">
         <v>10</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S18" s="4">
         <v>2</v>
       </c>
       <c r="T18" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -2399,49 +2428,49 @@
         <v>2</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>39</v>
+        <v>232</v>
       </c>
       <c r="H19" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="J19" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="I19" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="J19" s="4" t="s">
+      <c r="K19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="K19" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L19" s="4" t="s">
+      <c r="M19" s="4">
+        <v>2</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O19" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="M19" s="4">
-        <v>2</v>
-      </c>
-      <c r="N19" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="O19" s="4" t="s">
+      <c r="P19" s="4" t="s">
         <v>181</v>
-      </c>
-      <c r="P19" s="4" t="s">
-        <v>182</v>
       </c>
       <c r="Q19" s="4">
         <v>10</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S19" s="4">
         <v>2</v>
       </c>
       <c r="T19" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -2467,46 +2496,46 @@
         <v>28</v>
       </c>
       <c r="H20" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="I20" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="J20" s="4" t="s">
+      <c r="K20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L20" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="K20" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L20" s="4" t="s">
+      <c r="M20" s="4">
+        <v>1</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="O20" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="M20" s="4">
-        <v>1</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="O20" s="4" t="s">
-        <v>186</v>
-      </c>
       <c r="P20" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q20" s="4">
         <v>20</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S20" s="4">
         <v>0</v>
       </c>
       <c r="T20" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -2532,46 +2561,46 @@
         <v>29</v>
       </c>
       <c r="H21" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="I21" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="J21" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="K21" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="K21" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L21" s="4" t="s">
+      <c r="M21" s="4">
+        <v>1</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O21" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="M21" s="4">
-        <v>1</v>
-      </c>
-      <c r="N21" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="O21" s="4" t="s">
-        <v>192</v>
-      </c>
       <c r="P21" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q21" s="4">
         <v>9</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S21" s="4">
         <v>0</v>
       </c>
       <c r="T21" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -2597,46 +2626,46 @@
         <v>30</v>
       </c>
       <c r="H22" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="J22" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="J22" s="4" t="s">
+      <c r="K22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L22" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="K22" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L22" s="4" t="s">
+      <c r="M22" s="4">
+        <v>1</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O22" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="M22" s="4">
-        <v>1</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="O22" s="4" t="s">
-        <v>196</v>
-      </c>
       <c r="P22" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q22" s="4">
         <v>0</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S22" s="4">
         <v>0</v>
       </c>
       <c r="T22" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -2662,46 +2691,46 @@
         <v>31</v>
       </c>
       <c r="H23" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="I23" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="J23" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="K23" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L23" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="K23" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L23" s="4" t="s">
+      <c r="M23" s="4">
+        <v>1</v>
+      </c>
+      <c r="N23" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="M23" s="4">
-        <v>1</v>
-      </c>
-      <c r="N23" s="4" t="s">
+      <c r="O23" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="O23" s="4" t="s">
-        <v>202</v>
-      </c>
       <c r="P23" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q23" s="4">
         <v>20</v>
       </c>
       <c r="R23" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S23" s="4">
         <v>0</v>
       </c>
       <c r="T23" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -2724,49 +2753,49 @@
         <v>2</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H24" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="J24" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="J24" s="4" t="s">
+      <c r="K24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L24" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="K24" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>206</v>
-      </c>
       <c r="M24" s="4">
         <v>1</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P24" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q24" s="4">
         <v>10</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S24" s="4">
         <v>1</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -2792,76 +2821,76 @@
         <v>32</v>
       </c>
       <c r="H25" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="J25" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="J25" s="4" t="s">
+      <c r="K25" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L25" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="K25" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L25" s="4" t="s">
+      <c r="M25" s="4">
+        <v>2</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O25" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="M25" s="4">
-        <v>2</v>
-      </c>
-      <c r="N25" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="O25" s="4" t="s">
-        <v>210</v>
-      </c>
       <c r="P25" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q25" s="4">
         <v>10</v>
       </c>
       <c r="R25" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S25" s="4">
         <v>2</v>
       </c>
       <c r="T25" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:21">
       <c r="B26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:21">
       <c r="B27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:21">
       <c r="D28" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2896,92 +2925,92 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Forgot to upload new input file
monoistのURL解析がいけたので変更。
(pagenum)となっていたものをreplaceしなくてよいように変更。
reportファイルは情報共有用。
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACS-NOSE\ANAtrial_nose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B197C473-F157-4FBC-AF3B-766EB1C7ABA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56A4AFF-E86A-49C8-9065-D474064EEDBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,9 +154,6 @@
     <t>https://ainow.ai/?s=(keyword)</t>
   </si>
   <si>
-    <t>https://gigazine.net/search/results/(keyword)/</t>
-  </si>
-  <si>
     <t>https://kyodonewsprwire.jp/search?s=(keyword)</t>
   </si>
   <si>
@@ -809,31 +806,35 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>https://robotstart.info/?paged=(pagenum)&amp;s=(keyword)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>https://sorae.info/?s=(keyword)&amp;paged=(pagenum)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>https://techable.jp/page/(pagenum)/?s=(keyword)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>https://wirelesswire.jp/page/(pagenum)/?s=(keyword)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>https://www.moguravr.com/page/(pagenum)/?s=(keyword)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>https://cse.google.co.jp/cse?cx=partner-pub-2201843946232317:9909425848&amp;q=(keyword)&amp;oq=(keyword)&amp;gs_l=partner-generic.3...9274.9387.0.10069.2.2.0.0.0.0.59.103.2.2.0.gsnos%2Cn%3D13...0.44j976j3..1ac.1.25.partner-generic..1.1.59.hWZNG5ZBd8A</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://gigazine.net</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://robotstart.info/?paged=1&amp;s=(keyword)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://techable.jp/page/1/?s=(keyword)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://sorae.info/?s=(keyword)&amp;paged=1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://wirelesswire.jp/page/1/?s=(keyword)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://www.moguravr.com/page/1/?s=(keyword)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -913,13 +914,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1240,67 +1242,67 @@
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" ht="18">
       <c r="A1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="D1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>215</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="T1" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="U1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -1326,46 +1328,46 @@
         <v>33</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="K2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4">
+        <v>2</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="M2" s="4">
-        <v>2</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="Q2" s="4">
         <v>20</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S2" s="4">
         <v>0</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -1387,50 +1389,50 @@
       <c r="F3" s="4">
         <v>1</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>34</v>
+      <c r="G3" s="6" t="s">
+        <v>228</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4">
+        <v>1</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="M3" s="4">
-        <v>1</v>
-      </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="Q3" s="4">
         <v>50</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S3" s="4">
         <v>0</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -1453,49 +1455,49 @@
         <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="M4" s="4">
+        <v>2</v>
+      </c>
+      <c r="N4" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="M4" s="4">
-        <v>2</v>
-      </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="O4" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="P4" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q4" s="4">
         <v>25</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S4" s="4">
         <v>0</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -1518,49 +1520,49 @@
         <v>1</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H5" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="4">
+        <v>1</v>
+      </c>
+      <c r="N5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="M5" s="4">
-        <v>1</v>
-      </c>
-      <c r="N5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="Q5" s="4">
         <v>30</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S5" s="4">
         <v>0</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -1583,49 +1585,49 @@
         <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H6" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="K6" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L6" s="4" t="s">
+      <c r="M6" s="4">
+        <v>1</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="O6" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="4">
-        <v>1</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="O6" s="4" t="s">
+      <c r="P6" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="Q6" s="4">
         <v>21</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S6" s="4">
         <v>0</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -1648,49 +1650,49 @@
         <v>1</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="J7" s="4" t="s">
+      <c r="K7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L7" s="4" t="s">
+      <c r="M7" s="4">
+        <v>1</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="O7" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="M7" s="4">
-        <v>1</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="P7" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q7" s="4">
         <v>20</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S7" s="4">
         <v>0</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -1713,49 +1715,49 @@
         <v>1</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H8" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="K8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L8" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L8" s="4" t="s">
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="O8" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="M8" s="4">
-        <v>1</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>122</v>
-      </c>
       <c r="P8" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q8" s="4">
         <v>10</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S8" s="4">
         <v>0</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1778,49 +1780,49 @@
         <v>2</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H9" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="J9" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="K9" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L9" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="K9" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L9" s="4" t="s">
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
+      <c r="N9" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="M9" s="4">
-        <v>1</v>
-      </c>
-      <c r="N9" s="4" t="s">
+      <c r="O9" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="O9" s="4" t="s">
-        <v>128</v>
-      </c>
       <c r="P9" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q9" s="4">
         <v>15</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S9" s="4">
         <v>0</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -1843,49 +1845,49 @@
         <v>2</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="H10" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="J10" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="K10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="K10" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L10" s="4" t="s">
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+      <c r="N10" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="M10" s="4">
-        <v>1</v>
-      </c>
-      <c r="N10" s="4" t="s">
+      <c r="O10" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="O10" s="4" t="s">
-        <v>134</v>
-      </c>
       <c r="P10" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q10" s="4">
         <v>10</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S10" s="4">
         <v>0</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1908,49 +1910,49 @@
         <v>2</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H11" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="K11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="K11" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L11" s="4" t="s">
+      <c r="M11" s="4">
+        <v>2</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O11" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="M11" s="4">
-        <v>2</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>139</v>
-      </c>
       <c r="P11" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q11" s="4">
         <v>14</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S11" s="4">
         <v>0</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1973,49 +1975,49 @@
         <v>2</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="H12" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="J12" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="K12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="K12" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L12" s="4" t="s">
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O12" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="M12" s="4">
-        <v>1</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>144</v>
-      </c>
       <c r="P12" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q12" s="4">
         <v>20</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S12" s="4">
         <v>0</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -2038,49 +2040,49 @@
         <v>2</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="H13" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="J13" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="K13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="K13" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L13" s="4" t="s">
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O13" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="M13" s="4">
-        <v>1</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="P13" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q13" s="4">
         <v>16</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S13" s="4">
         <v>0</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -2106,46 +2108,46 @@
         <v>24</v>
       </c>
       <c r="H14" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J14" s="4" t="s">
+      <c r="K14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L14" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="K14" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L14" s="4" t="s">
+      <c r="M14" s="4">
+        <v>1</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="O14" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M14" s="4">
-        <v>1</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>153</v>
-      </c>
       <c r="P14" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q14" s="4">
         <v>10</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S14" s="4">
         <v>2</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -2165,52 +2167,52 @@
         <v>1</v>
       </c>
       <c r="F15" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="H15" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="J15" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="K15" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="L15" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="M15" s="4">
+        <v>2</v>
+      </c>
+      <c r="N15" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="M15" s="4">
-        <v>2</v>
-      </c>
-      <c r="N15" s="4" t="s">
+      <c r="O15" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="O15" s="4" t="s">
-        <v>161</v>
-      </c>
       <c r="P15" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q15" s="4">
         <v>10</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S15" s="4">
         <v>0</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -2236,46 +2238,46 @@
         <v>26</v>
       </c>
       <c r="H16" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="I16" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="J16" s="4" t="s">
+      <c r="K16" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="K16" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L16" s="4" t="s">
+      <c r="M16" s="4">
+        <v>2</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="O16" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="M16" s="4">
-        <v>2</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>166</v>
-      </c>
       <c r="P16" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q16" s="4">
         <v>50</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S16" s="4">
         <v>0</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -2283,7 +2285,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4">
         <v>0</v>
@@ -2298,49 +2300,49 @@
         <v>2</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H17" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="J17" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="I17" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="J17" s="4" t="s">
+      <c r="K17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="K17" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L17" s="4" t="s">
+      <c r="M17" s="4">
+        <v>1</v>
+      </c>
+      <c r="N17" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="M17" s="4">
-        <v>1</v>
-      </c>
-      <c r="N17" s="4" t="s">
+      <c r="O17" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="O17" s="4" t="s">
-        <v>171</v>
-      </c>
       <c r="P17" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q17" s="4">
         <v>10</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S17" s="4">
         <v>0</v>
       </c>
       <c r="T17" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -2366,46 +2368,46 @@
         <v>27</v>
       </c>
       <c r="H18" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="J18" s="4" t="s">
+      <c r="K18" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L18" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="K18" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L18" s="4" t="s">
+      <c r="M18" s="4">
+        <v>1</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="O18" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="M18" s="4">
-        <v>1</v>
-      </c>
-      <c r="N18" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O18" s="4" t="s">
-        <v>176</v>
-      </c>
       <c r="P18" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q18" s="4">
         <v>10</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S18" s="4">
         <v>2</v>
       </c>
       <c r="T18" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -2428,49 +2430,49 @@
         <v>2</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="H19" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="J19" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="I19" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="J19" s="4" t="s">
+      <c r="K19" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="K19" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L19" s="4" t="s">
+      <c r="M19" s="4">
+        <v>2</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="O19" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="M19" s="4">
-        <v>2</v>
-      </c>
-      <c r="N19" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O19" s="4" t="s">
+      <c r="P19" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="P19" s="4" t="s">
-        <v>181</v>
       </c>
       <c r="Q19" s="4">
         <v>10</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S19" s="4">
         <v>2</v>
       </c>
       <c r="T19" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -2496,46 +2498,46 @@
         <v>28</v>
       </c>
       <c r="H20" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="I20" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="J20" s="4" t="s">
+      <c r="K20" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L20" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="K20" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L20" s="4" t="s">
+      <c r="M20" s="4">
+        <v>1</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="O20" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="M20" s="4">
-        <v>1</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="O20" s="4" t="s">
-        <v>185</v>
-      </c>
       <c r="P20" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q20" s="4">
         <v>20</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S20" s="4">
         <v>0</v>
       </c>
       <c r="T20" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -2561,46 +2563,46 @@
         <v>29</v>
       </c>
       <c r="H21" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="I21" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="J21" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="K21" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="K21" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L21" s="4" t="s">
+      <c r="M21" s="4">
+        <v>1</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="O21" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="M21" s="4">
-        <v>1</v>
-      </c>
-      <c r="N21" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O21" s="4" t="s">
-        <v>191</v>
-      </c>
       <c r="P21" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q21" s="4">
         <v>9</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S21" s="4">
         <v>0</v>
       </c>
       <c r="T21" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -2626,46 +2628,46 @@
         <v>30</v>
       </c>
       <c r="H22" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J22" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="J22" s="4" t="s">
+      <c r="K22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L22" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="K22" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L22" s="4" t="s">
+      <c r="M22" s="4">
+        <v>1</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="O22" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="M22" s="4">
-        <v>1</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O22" s="4" t="s">
-        <v>195</v>
-      </c>
       <c r="P22" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q22" s="4">
         <v>0</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S22" s="4">
         <v>0</v>
       </c>
       <c r="T22" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -2691,46 +2693,46 @@
         <v>31</v>
       </c>
       <c r="H23" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="I23" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="J23" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="K23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L23" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="K23" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L23" s="4" t="s">
+      <c r="M23" s="4">
+        <v>1</v>
+      </c>
+      <c r="N23" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="M23" s="4">
-        <v>1</v>
-      </c>
-      <c r="N23" s="4" t="s">
+      <c r="O23" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="O23" s="4" t="s">
-        <v>201</v>
-      </c>
       <c r="P23" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q23" s="4">
         <v>20</v>
       </c>
       <c r="R23" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S23" s="4">
         <v>0</v>
       </c>
       <c r="T23" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -2738,7 +2740,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="4">
         <v>0</v>
@@ -2753,49 +2755,49 @@
         <v>2</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H24" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="J24" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="J24" s="4" t="s">
+      <c r="K24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L24" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="K24" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>205</v>
-      </c>
       <c r="M24" s="4">
         <v>1</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P24" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q24" s="4">
         <v>10</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S24" s="4">
         <v>1</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -2821,76 +2823,76 @@
         <v>32</v>
       </c>
       <c r="H25" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="J25" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="J25" s="4" t="s">
+      <c r="K25" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L25" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="K25" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L25" s="4" t="s">
+      <c r="M25" s="4">
+        <v>2</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="O25" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="M25" s="4">
-        <v>2</v>
-      </c>
-      <c r="N25" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O25" s="4" t="s">
-        <v>209</v>
-      </c>
       <c r="P25" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q25" s="4">
         <v>10</v>
       </c>
       <c r="R25" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S25" s="4">
         <v>2</v>
       </c>
       <c r="T25" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="26" spans="1:21">
       <c r="B26" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:21">
       <c r="B27" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:21">
       <c r="D28" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2925,92 +2927,92 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Excel sheet:"console" (avoid to change source code -> the part of inputting file)
テストの際に意図的にキーワード数を減らしてソースコードを書き換えることが多いので、すべてExcelファイルでの管理に変更しました。
これにより実行時に直接ソースコードをいじることがなくなり不測の事態を避けられます。
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACS-NOSE\ANAtrial_nose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3937A8D2-5DCB-468B-9D39-E25DA612DC54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90436DC9-641B-4507-B3C8-100FC8F96B72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="URL" sheetId="1" r:id="rId1"/>
-    <sheet name="keyword" sheetId="2" r:id="rId2"/>
+    <sheet name="console" sheetId="3" r:id="rId1"/>
+    <sheet name="website" sheetId="1" r:id="rId2"/>
+    <sheet name="keyword" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="250">
   <si>
     <t>ascii</t>
     <phoneticPr fontId="1"/>
@@ -872,6 +873,34 @@
   </si>
   <si>
     <t>5s</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KeywordName</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■Crawling Keyword</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■Crawling Website</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>StartWebsite Row No.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FinishWebsite Row No.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>StartKeyword Row No.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FinishKeyword Row No.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -913,13 +942,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -951,16 +980,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1263,1827 +1293,1887 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F5DE21E-C6D9-4593-875A-5722EF796782}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <cols>
+    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B7" s="2">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.75" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="56.75" style="2" customWidth="1"/>
-    <col min="10" max="16" width="9" style="2"/>
-    <col min="17" max="17" width="30.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.75" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="56.75" style="1" customWidth="1"/>
+    <col min="10" max="16" width="9" style="1"/>
+    <col min="17" max="17" width="30.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="18">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:23" s="7" customFormat="1" ht="18">
+      <c r="A1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="7" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:23">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>1</v>
-      </c>
-      <c r="E2" s="6">
-        <v>1</v>
-      </c>
-      <c r="F2" s="6">
-        <v>1</v>
-      </c>
-      <c r="G2" s="6" t="s">
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="M2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="O2" s="4">
-        <v>2</v>
-      </c>
-      <c r="P2" s="4" t="s">
+      <c r="O2" s="2">
+        <v>2</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="S2" s="4">
+      <c r="S2" s="2">
         <v>20</v>
       </c>
-      <c r="T2" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U2" s="4">
-        <v>0</v>
-      </c>
-      <c r="V2" s="4" t="s">
+      <c r="T2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U2" s="2">
+        <v>0</v>
+      </c>
+      <c r="V2" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" s="1" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:23">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-      <c r="F3" s="6">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="M3" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N3" s="4" t="s">
+      <c r="M3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="O3" s="4">
-        <v>1</v>
-      </c>
-      <c r="P3" s="4" t="s">
+      <c r="O3" s="2">
+        <v>1</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="S3" s="4">
+      <c r="S3" s="2">
         <v>50</v>
       </c>
-      <c r="T3" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U3" s="4">
-        <v>0</v>
-      </c>
-      <c r="V3" s="4" t="s">
+      <c r="T3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0</v>
+      </c>
+      <c r="V3" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="W3" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:23">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1</v>
-      </c>
-      <c r="E4" s="6">
-        <v>1</v>
-      </c>
-      <c r="F4" s="6">
-        <v>1</v>
-      </c>
-      <c r="G4" s="6" t="s">
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="O4" s="4">
-        <v>2</v>
-      </c>
-      <c r="P4" s="4" t="s">
+      <c r="O4" s="2">
+        <v>2</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="S4" s="4">
+      <c r="S4" s="2">
         <v>25</v>
       </c>
-      <c r="T4" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U4" s="4">
-        <v>0</v>
-      </c>
-      <c r="V4" s="4" t="s">
+      <c r="T4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0</v>
+      </c>
+      <c r="V4" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="W4" s="1" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:23">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="6">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6">
-        <v>1</v>
-      </c>
-      <c r="F5" s="6">
-        <v>1</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N5" s="4" t="s">
+      <c r="M5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="O5" s="4">
-        <v>1</v>
-      </c>
-      <c r="P5" s="4" t="s">
+      <c r="O5" s="2">
+        <v>1</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="Q5" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="S5" s="4">
+      <c r="S5" s="2">
         <v>30</v>
       </c>
-      <c r="T5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U5" s="4">
-        <v>0</v>
-      </c>
-      <c r="V5" s="4" t="s">
+      <c r="T5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0</v>
+      </c>
+      <c r="V5" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="W5" s="1" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:23">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="6">
-        <v>2</v>
-      </c>
-      <c r="F6" s="6">
-        <v>1</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="M6" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N6" s="4" t="s">
+      <c r="M6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="O6" s="4">
-        <v>1</v>
-      </c>
-      <c r="P6" s="4" t="s">
+      <c r="O6" s="2">
+        <v>1</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="Q6" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="R6" s="4" t="s">
+      <c r="R6" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="S6" s="4">
+      <c r="S6" s="2">
         <v>21</v>
       </c>
-      <c r="T6" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U6" s="4">
-        <v>0</v>
-      </c>
-      <c r="V6" s="4" t="s">
+      <c r="T6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0</v>
+      </c>
+      <c r="V6" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="W6" s="2" t="s">
+      <c r="W6" s="1" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:23">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="6">
-        <v>0</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6">
-        <v>1</v>
-      </c>
-      <c r="E7" s="6">
-        <v>2</v>
-      </c>
-      <c r="F7" s="6">
-        <v>1</v>
-      </c>
-      <c r="G7" s="6" t="s">
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="M7" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N7" s="4" t="s">
+      <c r="M7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="O7" s="4">
-        <v>1</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q7" s="4" t="s">
+      <c r="O7" s="2">
+        <v>1</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q7" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="R7" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="S7" s="4">
+      <c r="R7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S7" s="2">
         <v>20</v>
       </c>
-      <c r="T7" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U7" s="4">
-        <v>0</v>
-      </c>
-      <c r="V7" s="4" t="s">
+      <c r="T7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0</v>
+      </c>
+      <c r="V7" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="W7" s="1" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="6">
-        <v>0</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-      <c r="E8" s="6">
-        <v>1</v>
-      </c>
-      <c r="F8" s="6">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="M8" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N8" s="4" t="s">
+      <c r="M8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="O8" s="4">
-        <v>1</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q8" s="4" t="s">
+      <c r="O8" s="2">
+        <v>1</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q8" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="R8" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="S8" s="4">
+      <c r="R8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S8" s="2">
         <v>10</v>
       </c>
-      <c r="T8" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U8" s="4">
-        <v>0</v>
-      </c>
-      <c r="V8" s="4" t="s">
+      <c r="T8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0</v>
+      </c>
+      <c r="V8" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="W8" s="1" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="6">
-        <v>0</v>
-      </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6">
-        <v>1</v>
-      </c>
-      <c r="E9" s="6">
-        <v>1</v>
-      </c>
-      <c r="F9" s="6">
-        <v>2</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
+        <v>2</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="M9" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N9" s="4" t="s">
+      <c r="M9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N9" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="O9" s="4">
-        <v>1</v>
-      </c>
-      <c r="P9" s="4" t="s">
+      <c r="O9" s="2">
+        <v>1</v>
+      </c>
+      <c r="P9" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="Q9" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="R9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="S9" s="4">
+      <c r="S9" s="2">
         <v>15</v>
       </c>
-      <c r="T9" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U9" s="4">
-        <v>0</v>
-      </c>
-      <c r="V9" s="4" t="s">
+      <c r="T9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U9" s="2">
+        <v>0</v>
+      </c>
+      <c r="V9" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="W9" s="2" t="s">
+      <c r="W9" s="1" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="6">
-        <v>0</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6">
-        <v>1</v>
-      </c>
-      <c r="E10" s="6">
-        <v>1</v>
-      </c>
-      <c r="F10" s="6">
-        <v>2</v>
-      </c>
-      <c r="G10" s="6" t="s">
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
+        <v>2</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="M10" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N10" s="4" t="s">
+      <c r="M10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N10" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="O10" s="4">
-        <v>1</v>
-      </c>
-      <c r="P10" s="4" t="s">
+      <c r="O10" s="2">
+        <v>1</v>
+      </c>
+      <c r="P10" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="Q10" s="4" t="s">
+      <c r="Q10" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="R10" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="S10" s="4">
+      <c r="R10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S10" s="2">
         <v>10</v>
       </c>
-      <c r="T10" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U10" s="4">
-        <v>0</v>
-      </c>
-      <c r="V10" s="4" t="s">
+      <c r="T10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U10" s="2">
+        <v>0</v>
+      </c>
+      <c r="V10" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="W10" s="2" t="s">
+      <c r="W10" s="1" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="6">
-        <v>0</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
-        <v>1</v>
-      </c>
-      <c r="E11" s="6">
-        <v>2</v>
-      </c>
-      <c r="F11" s="6">
-        <v>2</v>
-      </c>
-      <c r="G11" s="6" t="s">
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="M11" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N11" s="4" t="s">
+      <c r="M11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N11" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="O11" s="4">
-        <v>2</v>
-      </c>
-      <c r="P11" s="4" t="s">
+      <c r="O11" s="2">
+        <v>2</v>
+      </c>
+      <c r="P11" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q11" s="4" t="s">
+      <c r="Q11" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="R11" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="S11" s="4">
+      <c r="S11" s="2">
         <v>14</v>
       </c>
-      <c r="T11" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U11" s="4">
-        <v>0</v>
-      </c>
-      <c r="V11" s="4" t="s">
+      <c r="T11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U11" s="2">
+        <v>0</v>
+      </c>
+      <c r="V11" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="W11" s="2" t="s">
+      <c r="W11" s="1" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="6">
-        <v>0</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
-        <v>1</v>
-      </c>
-      <c r="E12" s="6">
-        <v>1</v>
-      </c>
-      <c r="F12" s="6">
-        <v>2</v>
-      </c>
-      <c r="G12" s="6" t="s">
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
+        <v>2</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="M12" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N12" s="4" t="s">
+      <c r="M12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="O12" s="4">
-        <v>1</v>
-      </c>
-      <c r="P12" s="4" t="s">
+      <c r="O12" s="2">
+        <v>1</v>
+      </c>
+      <c r="P12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q12" s="4" t="s">
+      <c r="Q12" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="R12" s="4" t="s">
+      <c r="R12" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="S12" s="4">
+      <c r="S12" s="2">
         <v>20</v>
       </c>
-      <c r="T12" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U12" s="4">
-        <v>0</v>
-      </c>
-      <c r="V12" s="4" t="s">
+      <c r="T12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U12" s="2">
+        <v>0</v>
+      </c>
+      <c r="V12" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="W12" s="2" t="s">
+      <c r="W12" s="1" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:23">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="6">
-        <v>0</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1</v>
-      </c>
-      <c r="E13" s="6">
-        <v>1</v>
-      </c>
-      <c r="F13" s="6">
-        <v>2</v>
-      </c>
-      <c r="G13" s="6" t="s">
+      <c r="B13" s="4">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4">
+        <v>2</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="M13" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N13" s="4" t="s">
+      <c r="M13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N13" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="O13" s="4">
-        <v>1</v>
-      </c>
-      <c r="P13" s="4" t="s">
+      <c r="O13" s="2">
+        <v>1</v>
+      </c>
+      <c r="P13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q13" s="4" t="s">
+      <c r="Q13" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="R13" s="4" t="s">
+      <c r="R13" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="S13" s="4">
+      <c r="S13" s="2">
         <v>16</v>
       </c>
-      <c r="T13" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U13" s="4">
-        <v>0</v>
-      </c>
-      <c r="V13" s="4" t="s">
+      <c r="T13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U13" s="2">
+        <v>0</v>
+      </c>
+      <c r="V13" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="W13" s="2" t="s">
+      <c r="W13" s="1" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:23">
-      <c r="A14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="6">
-        <v>0</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0</v>
-      </c>
-      <c r="D14" s="6">
-        <v>2</v>
-      </c>
-      <c r="E14" s="6">
-        <v>1</v>
-      </c>
-      <c r="F14" s="6">
-        <v>2</v>
-      </c>
-      <c r="G14" s="6" t="s">
+      <c r="A14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4">
+        <v>2</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="M14" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N14" s="4" t="s">
+      <c r="M14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N14" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="O14" s="4">
-        <v>1</v>
-      </c>
-      <c r="P14" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q14" s="4" t="s">
+      <c r="O14" s="2">
+        <v>1</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q14" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="R14" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="S14" s="4">
+      <c r="R14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S14" s="2">
         <v>10</v>
       </c>
-      <c r="T14" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U14" s="4">
-        <v>2</v>
-      </c>
-      <c r="V14" s="4" t="s">
+      <c r="T14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U14" s="2">
+        <v>2</v>
+      </c>
+      <c r="V14" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="W14" s="2" t="s">
+      <c r="W14" s="1" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:23">
-      <c r="A15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="6">
-        <v>0</v>
-      </c>
-      <c r="C15" s="6">
-        <v>0</v>
-      </c>
-      <c r="D15" s="6">
-        <v>2</v>
-      </c>
-      <c r="E15" s="6">
-        <v>1</v>
-      </c>
-      <c r="F15" s="6">
-        <v>1</v>
-      </c>
-      <c r="G15" s="6" t="s">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="L15" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="M15" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="N15" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="O15" s="4">
-        <v>2</v>
-      </c>
-      <c r="P15" s="4" t="s">
+      <c r="O15" s="2">
+        <v>2</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q15" s="4" t="s">
+      <c r="Q15" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="R15" s="4" t="s">
+      <c r="R15" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="S15" s="4">
+      <c r="S15" s="2">
         <v>10</v>
       </c>
-      <c r="T15" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U15" s="4">
-        <v>0</v>
-      </c>
-      <c r="V15" s="4" t="s">
+      <c r="T15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U15" s="2">
+        <v>0</v>
+      </c>
+      <c r="V15" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="W15" s="2" t="s">
+      <c r="W15" s="1" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="6">
-        <v>0</v>
-      </c>
-      <c r="C16" s="6">
-        <v>0</v>
-      </c>
-      <c r="D16" s="6">
-        <v>2</v>
-      </c>
-      <c r="E16" s="6">
-        <v>1</v>
-      </c>
-      <c r="F16" s="6">
-        <v>1</v>
-      </c>
-      <c r="G16" s="6" t="s">
+      <c r="A16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="L16" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="M16" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N16" s="4" t="s">
+      <c r="M16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N16" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="O16" s="4">
-        <v>2</v>
-      </c>
-      <c r="P16" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q16" s="4" t="s">
+      <c r="O16" s="2">
+        <v>2</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q16" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="R16" s="4" t="s">
+      <c r="R16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="S16" s="4">
+      <c r="S16" s="2">
         <v>50</v>
       </c>
-      <c r="T16" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U16" s="4">
-        <v>0</v>
-      </c>
-      <c r="V16" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="W16" s="2" t="s">
+      <c r="T16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U16" s="2">
+        <v>0</v>
+      </c>
+      <c r="V16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W16" s="1" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:23">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="6">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6">
-        <v>0</v>
-      </c>
-      <c r="D17" s="6">
-        <v>2</v>
-      </c>
-      <c r="E17" s="6">
-        <v>1</v>
-      </c>
-      <c r="F17" s="6">
-        <v>2</v>
-      </c>
-      <c r="G17" s="6" t="s">
+      <c r="B17" s="4">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4">
+        <v>2</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="L17" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="M17" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N17" s="4" t="s">
+      <c r="M17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N17" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="O17" s="4">
-        <v>1</v>
-      </c>
-      <c r="P17" s="4" t="s">
+      <c r="O17" s="2">
+        <v>1</v>
+      </c>
+      <c r="P17" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="Q17" s="4" t="s">
+      <c r="Q17" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="R17" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="S17" s="4">
+      <c r="R17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S17" s="2">
         <v>10</v>
       </c>
-      <c r="T17" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U17" s="4">
-        <v>0</v>
-      </c>
-      <c r="V17" s="4" t="s">
+      <c r="T17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U17" s="2">
+        <v>0</v>
+      </c>
+      <c r="V17" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="W17" s="2" t="s">
+      <c r="W17" s="1" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:23">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="6">
-        <v>0</v>
-      </c>
-      <c r="C18" s="6">
-        <v>0</v>
-      </c>
-      <c r="D18" s="6">
-        <v>2</v>
-      </c>
-      <c r="E18" s="6">
-        <v>1</v>
-      </c>
-      <c r="F18" s="6">
-        <v>1</v>
-      </c>
-      <c r="G18" s="6" t="s">
+      <c r="B18" s="4">
+        <v>0</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>2</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="L18" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="M18" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N18" s="4" t="s">
+      <c r="M18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N18" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="O18" s="4">
-        <v>1</v>
-      </c>
-      <c r="P18" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q18" s="4" t="s">
+      <c r="O18" s="2">
+        <v>1</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q18" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="R18" s="4" t="s">
+      <c r="R18" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="S18" s="4">
+      <c r="S18" s="2">
         <v>10</v>
       </c>
-      <c r="T18" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U18" s="4">
-        <v>2</v>
-      </c>
-      <c r="V18" s="4" t="s">
+      <c r="T18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U18" s="2">
+        <v>2</v>
+      </c>
+      <c r="V18" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="W18" s="2" t="s">
+      <c r="W18" s="1" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:23">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="6">
-        <v>0</v>
-      </c>
-      <c r="C19" s="6">
-        <v>0</v>
-      </c>
-      <c r="D19" s="6">
-        <v>2</v>
-      </c>
-      <c r="E19" s="6">
-        <v>1</v>
-      </c>
-      <c r="F19" s="6">
-        <v>2</v>
-      </c>
-      <c r="G19" s="6" t="s">
+      <c r="B19" s="4">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4">
+        <v>2</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="L19" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="M19" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N19" s="4" t="s">
+      <c r="M19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N19" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="O19" s="4">
-        <v>2</v>
-      </c>
-      <c r="P19" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q19" s="4" t="s">
+      <c r="O19" s="2">
+        <v>2</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q19" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="R19" s="4" t="s">
+      <c r="R19" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="S19" s="4">
+      <c r="S19" s="2">
         <v>10</v>
       </c>
-      <c r="T19" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U19" s="4">
-        <v>2</v>
-      </c>
-      <c r="V19" s="4" t="s">
+      <c r="T19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U19" s="2">
+        <v>2</v>
+      </c>
+      <c r="V19" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="W19" s="2" t="s">
+      <c r="W19" s="1" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:23">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="6">
-        <v>0</v>
-      </c>
-      <c r="C20" s="6">
-        <v>0</v>
-      </c>
-      <c r="D20" s="6">
-        <v>2</v>
-      </c>
-      <c r="E20" s="6">
-        <v>2</v>
-      </c>
-      <c r="F20" s="6">
-        <v>1</v>
-      </c>
-      <c r="G20" s="6" t="s">
+      <c r="B20" s="4">
+        <v>0</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2</v>
+      </c>
+      <c r="E20" s="4">
+        <v>2</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="L20" s="4" t="s">
+      <c r="L20" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="M20" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N20" s="4" t="s">
+      <c r="M20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N20" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="O20" s="4">
-        <v>1</v>
-      </c>
-      <c r="P20" s="4" t="s">
+      <c r="O20" s="2">
+        <v>1</v>
+      </c>
+      <c r="P20" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q20" s="4" t="s">
+      <c r="Q20" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="R20" s="4" t="s">
+      <c r="R20" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="S20" s="4">
+      <c r="S20" s="2">
         <v>20</v>
       </c>
-      <c r="T20" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U20" s="4">
-        <v>0</v>
-      </c>
-      <c r="V20" s="4" t="s">
+      <c r="T20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U20" s="2">
+        <v>0</v>
+      </c>
+      <c r="V20" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="W20" s="2" t="s">
+      <c r="W20" s="1" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:23">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="6">
-        <v>0</v>
-      </c>
-      <c r="C21" s="6">
-        <v>0</v>
-      </c>
-      <c r="D21" s="6">
-        <v>2</v>
-      </c>
-      <c r="E21" s="6">
-        <v>2</v>
-      </c>
-      <c r="F21" s="6">
-        <v>1</v>
-      </c>
-      <c r="G21" s="6" t="s">
+      <c r="B21" s="4">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2</v>
+      </c>
+      <c r="E21" s="4">
+        <v>2</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="L21" s="4" t="s">
+      <c r="L21" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="M21" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N21" s="4" t="s">
+      <c r="M21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N21" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="O21" s="4">
-        <v>1</v>
-      </c>
-      <c r="P21" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q21" s="4" t="s">
+      <c r="O21" s="2">
+        <v>1</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q21" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="R21" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="S21" s="4">
+      <c r="R21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S21" s="2">
         <v>9</v>
       </c>
-      <c r="T21" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U21" s="4">
-        <v>0</v>
-      </c>
-      <c r="V21" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="W21" s="2" t="s">
+      <c r="T21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U21" s="2">
+        <v>0</v>
+      </c>
+      <c r="V21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W21" s="1" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:23">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="6">
-        <v>0</v>
-      </c>
-      <c r="C22" s="6">
-        <v>0</v>
-      </c>
-      <c r="D22" s="6">
-        <v>2</v>
-      </c>
-      <c r="E22" s="6">
-        <v>1</v>
-      </c>
-      <c r="F22" s="6">
-        <v>2</v>
-      </c>
-      <c r="G22" s="6" t="s">
+      <c r="B22" s="4">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4">
+        <v>2</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J22" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="L22" s="4" t="s">
+      <c r="L22" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="M22" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N22" s="4" t="s">
+      <c r="M22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N22" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="O22" s="4">
-        <v>1</v>
-      </c>
-      <c r="P22" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q22" s="4" t="s">
+      <c r="O22" s="2">
+        <v>1</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q22" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="R22" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="S22" s="4">
-        <v>0</v>
-      </c>
-      <c r="T22" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U22" s="4">
-        <v>0</v>
-      </c>
-      <c r="V22" s="4" t="s">
+      <c r="R22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S22" s="2">
+        <v>0</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U22" s="2">
+        <v>0</v>
+      </c>
+      <c r="V22" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="W22" s="2" t="s">
+      <c r="W22" s="1" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:23">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="6">
-        <v>0</v>
-      </c>
-      <c r="C23" s="6">
-        <v>0</v>
-      </c>
-      <c r="D23" s="6">
-        <v>2</v>
-      </c>
-      <c r="E23" s="6">
-        <v>1</v>
-      </c>
-      <c r="F23" s="6">
-        <v>1</v>
-      </c>
-      <c r="G23" s="6" t="s">
+      <c r="B23" s="4">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
+      <c r="F23" s="4">
+        <v>1</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K23" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="L23" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="M23" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N23" s="4" t="s">
+      <c r="M23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N23" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="O23" s="4">
-        <v>1</v>
-      </c>
-      <c r="P23" s="4" t="s">
+      <c r="O23" s="2">
+        <v>1</v>
+      </c>
+      <c r="P23" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="Q23" s="4" t="s">
+      <c r="Q23" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="R23" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="S23" s="4">
+      <c r="R23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S23" s="2">
         <v>20</v>
       </c>
-      <c r="T23" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U23" s="4">
-        <v>0</v>
-      </c>
-      <c r="V23" s="4" t="s">
+      <c r="T23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U23" s="2">
+        <v>0</v>
+      </c>
+      <c r="V23" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="W23" s="2" t="s">
+      <c r="W23" s="1" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:23">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="6">
-        <v>0</v>
-      </c>
-      <c r="C24" s="6">
-        <v>0</v>
-      </c>
-      <c r="D24" s="6">
-        <v>2</v>
-      </c>
-      <c r="E24" s="6">
-        <v>2</v>
-      </c>
-      <c r="F24" s="6">
-        <v>2</v>
-      </c>
-      <c r="G24" s="6" t="s">
+      <c r="B24" s="4">
+        <v>0</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>2</v>
+      </c>
+      <c r="E24" s="4">
+        <v>2</v>
+      </c>
+      <c r="F24" s="4">
+        <v>2</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H24" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="I24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="J24" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="K24" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="L24" s="4" t="s">
+      <c r="L24" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="M24" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N24" s="4" t="s">
+      <c r="M24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N24" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="O24" s="4">
-        <v>1</v>
-      </c>
-      <c r="P24" s="4" t="s">
+      <c r="O24" s="2">
+        <v>1</v>
+      </c>
+      <c r="P24" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q24" s="4" t="s">
+      <c r="Q24" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="R24" s="4" t="s">
+      <c r="R24" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="S24" s="4">
+      <c r="S24" s="2">
         <v>10</v>
       </c>
-      <c r="T24" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U24" s="4">
-        <v>1</v>
-      </c>
-      <c r="V24" s="4" t="s">
+      <c r="T24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U24" s="2">
+        <v>1</v>
+      </c>
+      <c r="V24" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="W24" s="2" t="s">
+      <c r="W24" s="1" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:23">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="6">
-        <v>0</v>
-      </c>
-      <c r="C25" s="6">
-        <v>0</v>
-      </c>
-      <c r="D25" s="6">
-        <v>2</v>
-      </c>
-      <c r="E25" s="6">
-        <v>1</v>
-      </c>
-      <c r="F25" s="6">
-        <v>2</v>
-      </c>
-      <c r="G25" s="6" t="s">
+      <c r="B25" s="4">
+        <v>0</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>2</v>
+      </c>
+      <c r="E25" s="4">
+        <v>1</v>
+      </c>
+      <c r="F25" s="4">
+        <v>2</v>
+      </c>
+      <c r="G25" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H25" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="I25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="J25" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="K25" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="L25" s="4" t="s">
+      <c r="L25" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="M25" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N25" s="4" t="s">
+      <c r="M25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N25" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="O25" s="4">
-        <v>2</v>
-      </c>
-      <c r="P25" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q25" s="4" t="s">
+      <c r="O25" s="2">
+        <v>2</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q25" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="R25" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="S25" s="4">
+      <c r="R25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S25" s="2">
         <v>10</v>
       </c>
-      <c r="T25" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U25" s="4">
-        <v>2</v>
-      </c>
-      <c r="V25" s="4" t="s">
+      <c r="T25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U25" s="2">
+        <v>2</v>
+      </c>
+      <c r="V25" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="W25" s="2" t="s">
+      <c r="W25" s="1" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:23">
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:23">
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="1" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3117,101 +3207,114 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEB8221F-E727-4C00-A892-93F8DA95C050}">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
+  <cols>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1">
+      <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1">
+      <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1">
+      <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1">
+      <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1">
+      <c r="A8" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1">
+      <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1">
+      <c r="A10" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1">
+      <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1">
+      <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
+    <row r="13" spans="1:1">
+      <c r="A13" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
+    <row r="14" spans="1:1">
+      <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
+    <row r="15" spans="1:1">
+      <c r="A15" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
+    <row r="16" spans="1:1">
+      <c r="A16" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+    <row r="19" spans="1:1">
+      <c r="A19" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Slight change for input file (monoist waittime)
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACS-NOSE\ANAtrial_nose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90436DC9-641B-4507-B3C8-100FC8F96B72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8696FCB8-C863-45A0-B6C0-43C7D7C74117}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="251">
   <si>
     <t>ascii</t>
     <phoneticPr fontId="1"/>
@@ -859,9 +859,6 @@
   </si>
   <si>
     <t>10s</t>
-  </si>
-  <si>
-    <t>10s</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -901,6 +898,14 @@
   </si>
   <si>
     <t>FinishKeyword Row No.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>7s</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>13s</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1296,7 +1301,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F5DE21E-C6D9-4593-875A-5722EF796782}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -1306,12 +1313,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B2" s="2">
         <v>2</v>
@@ -1319,7 +1326,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B3" s="2">
         <v>25</v>
@@ -1327,20 +1334,20 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B6" s="2">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B7" s="2">
         <v>19</v>
@@ -1349,6 +1356,7 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1465,7 +1473,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>237</v>
@@ -1536,7 +1544,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>237</v>
@@ -1607,7 +1615,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>237</v>
@@ -1678,7 +1686,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>237</v>
@@ -1749,10 +1757,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>232</v>
@@ -1820,10 +1828,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>231</v>
@@ -1891,7 +1899,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>236</v>
@@ -1962,7 +1970,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>236</v>
@@ -2033,7 +2041,7 @@
         <v>2</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>236</v>
@@ -2104,10 +2112,10 @@
         <v>2</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>223</v>
@@ -2175,7 +2183,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>236</v>
@@ -2246,7 +2254,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>236</v>
@@ -2317,10 +2325,10 @@
         <v>2</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>229</v>
@@ -2388,10 +2396,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>24</v>
@@ -2459,10 +2467,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>25</v>
@@ -2515,7 +2523,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4">
         <v>0</v>
@@ -2530,10 +2538,10 @@
         <v>2</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>230</v>
@@ -2601,10 +2609,10 @@
         <v>1</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>26</v>
@@ -2657,7 +2665,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="4">
         <v>0</v>
@@ -2672,10 +2680,10 @@
         <v>2</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>228</v>
@@ -2743,10 +2751,10 @@
         <v>1</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>27</v>
@@ -2814,10 +2822,10 @@
         <v>1</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>28</v>
@@ -2885,10 +2893,10 @@
         <v>2</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>29</v>
@@ -2956,10 +2964,10 @@
         <v>1</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>30</v>
@@ -3027,10 +3035,10 @@
         <v>2</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>36</v>
@@ -3098,10 +3106,10 @@
         <v>2</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>31</v>
@@ -3225,7 +3233,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:1">

</xml_diff>